<commit_message>
actualiza tus horas vivimos en una sociedad hijo de tu reputisima madre
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ DemoFinal.xlsx
+++ b/Documentación/To Do - Requisitos_ DemoFinal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golro\Documents\Universidad\año 3\primer cuatrimestre\IngenieriaDelSoftware\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC73E7-32CC-4505-9CCC-8C2797CEBCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7625029D-0581-426F-AC32-0DBAEAD544EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2933" yWindow="2933" windowWidth="19200" windowHeight="10074" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="224">
   <si>
     <t>Nombre</t>
   </si>
@@ -735,6 +735,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Apoyo RegistoUsuario</t>
   </si>
 </sst>
 </file>
@@ -820,7 +823,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -950,6 +953,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1104,7 +1113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1188,18 +1197,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1210,12 +1207,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1229,6 +1220,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1257,6 +1257,17 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2275,25 +2286,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P182"/>
+  <dimension ref="A2:P183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G167" sqref="G167"/>
+    <sheetView tabSelected="1" topLeftCell="A249" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.52734375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.453125" customWidth="1"/>
-    <col min="11" max="11" width="35.453125" customWidth="1"/>
-    <col min="12" max="12" width="26.54296875" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="5.52734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.52734375" customWidth="1"/>
+    <col min="5" max="5" width="13.52734375" customWidth="1"/>
+    <col min="7" max="7" width="53.46875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.46875" customWidth="1"/>
+    <col min="11" max="11" width="35.46875" customWidth="1"/>
+    <col min="12" max="12" width="26.52734375" customWidth="1"/>
+    <col min="16" max="16" width="17.46875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2328,15 +2339,15 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E998)</f>
-        <v>433.2</v>
+        <v>439.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>526.94999999999993</v>
+        <v>548.54999999999995</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="78">
+      <c r="K3" s="75">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145+J161</f>
         <v>141.25</v>
       </c>
@@ -2345,37 +2356,37 @@
       </c>
       <c r="M3">
         <f>K3+K6+K9+K12+K15+K18</f>
-        <v>522.95000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="63" t="s">
+        <v>541.55000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="78"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="78"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2390,10 +2401,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="62">
+      <c r="K6" s="69">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133+J148+J164</f>
         <v>91.320000000000007</v>
       </c>
@@ -2401,7 +2412,7 @@
       <c r="M6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -2416,13 +2427,13 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="62"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
@@ -2437,13 +2448,13 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="62"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
@@ -2458,17 +2469,17 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="62">
+      <c r="K9" s="69">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
         <v>114.78</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
@@ -2483,10 +2494,10 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="62"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="80"/>
+      <c r="K10" s="69"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -2501,12 +2512,12 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2521,15 +2532,15 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="62">
+      <c r="K12" s="69">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149+J165</f>
         <v>96.85</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
@@ -2544,10 +2555,10 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="62"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="64"/>
+      <c r="K13" s="69"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2562,10 +2573,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="62"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="65"/>
+      <c r="K14" s="69"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
@@ -2580,15 +2591,15 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="73" t="s">
+      <c r="J15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="62">
+      <c r="K15" s="69">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
@@ -2603,10 +2614,10 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="62"/>
-    </row>
-    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="71"/>
+      <c r="K16" s="69"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
@@ -2621,10 +2632,10 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="62"/>
-    </row>
-    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="72"/>
+      <c r="K17" s="69"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="10" t="s">
         <v>16</v>
       </c>
@@ -2641,15 +2652,15 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="76" t="s">
+      <c r="J18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="62">
-        <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
-        <v>36.75</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="69">
+        <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135+J150+J166</f>
+        <v>55.35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2667,10 +2678,10 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="62"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J19" s="74"/>
+      <c r="K19" s="69"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2687,10 +2698,10 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="62"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J20" s="74"/>
+      <c r="K20" s="69"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2708,7 +2719,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2725,13 +2736,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="72" t="s">
+      <c r="J22" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-    </row>
-    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+    </row>
+    <row r="23" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2749,7 +2760,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2767,7 +2778,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2785,7 +2796,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2803,7 +2814,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2821,7 +2832,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2839,7 +2850,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2857,7 +2868,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2875,7 +2886,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2892,7 +2903,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2910,7 +2921,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2926,7 +2937,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2944,7 +2955,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2962,7 +2973,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2980,7 +2991,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2998,7 +3009,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -3016,7 +3027,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -3034,7 +3045,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -3052,25 +3063,25 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="63" t="s">
+    <row r="41" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
-    </row>
-    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="65"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
-    </row>
-    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+    </row>
+    <row r="42" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+    </row>
+    <row r="43" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -3088,7 +3099,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -3106,7 +3117,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -3124,7 +3135,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -3142,7 +3153,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -3160,7 +3171,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -3178,7 +3189,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -3205,7 +3216,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -3234,7 +3245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -3263,7 +3274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -3292,7 +3303,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -3321,7 +3332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -3350,7 +3361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -3377,7 +3388,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -3395,7 +3406,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -3413,7 +3424,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -3440,7 +3451,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -3469,7 +3480,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -3498,7 +3509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3525,7 +3536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" s="4" t="s">
         <v>9</v>
       </c>
@@ -3554,7 +3565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B63" s="4" t="s">
         <v>9</v>
       </c>
@@ -3583,7 +3594,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B64" s="4" t="s">
         <v>9</v>
       </c>
@@ -3612,7 +3623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B65" s="4" t="s">
         <v>9</v>
       </c>
@@ -3630,7 +3641,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B66" s="6" t="s">
         <v>13</v>
       </c>
@@ -3649,7 +3660,7 @@
       </c>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B67" s="8" t="s">
         <v>14</v>
       </c>
@@ -3667,7 +3678,7 @@
       </c>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" s="8" t="s">
         <v>14</v>
       </c>
@@ -3685,7 +3696,7 @@
       </c>
       <c r="G68" s="26"/>
     </row>
-    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B69" s="10" t="s">
         <v>16</v>
       </c>
@@ -3703,7 +3714,7 @@
       </c>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B70" s="10" t="s">
         <v>16</v>
       </c>
@@ -3721,7 +3732,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
@@ -3739,15 +3750,15 @@
       </c>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="63" t="s">
+    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3758,13 +3769,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
+    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B73" s="61"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -3777,7 +3788,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B74" s="4" t="s">
         <v>9</v>
       </c>
@@ -3806,7 +3817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B75" s="5" t="s">
         <v>12</v>
       </c>
@@ -3835,7 +3846,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B76" s="9" t="s">
         <v>15</v>
       </c>
@@ -3862,7 +3873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B77" s="9" t="s">
         <v>15</v>
       </c>
@@ -3891,7 +3902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B78" s="9" t="s">
         <v>15</v>
       </c>
@@ -3913,14 +3924,14 @@
       </c>
       <c r="J78">
         <f>F79+F81+F82+F97+F121+F125+F126</f>
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="K78">
         <f>E79+E82+E81+E97+E121</f>
         <v>12.5</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B79" s="10" t="s">
         <v>16</v>
       </c>
@@ -3936,7 +3947,7 @@
       </c>
       <c r="G79" s="11"/>
     </row>
-    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B80" s="6" t="s">
         <v>13</v>
       </c>
@@ -3952,7 +3963,7 @@
       </c>
       <c r="G80" s="49"/>
     </row>
-    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B81" s="10" t="s">
         <v>16</v>
       </c>
@@ -3963,10 +3974,12 @@
       <c r="E81" s="34">
         <v>3</v>
       </c>
-      <c r="F81" s="34"/>
+      <c r="F81" s="34">
+        <v>1</v>
+      </c>
       <c r="G81" s="34"/>
     </row>
-    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B82" s="10" t="s">
         <v>16</v>
       </c>
@@ -3984,7 +3997,7 @@
       </c>
       <c r="G82" s="11"/>
     </row>
-    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B83" s="4" t="s">
         <v>9</v>
       </c>
@@ -4002,7 +4015,7 @@
       </c>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B84" s="8" t="s">
         <v>14</v>
       </c>
@@ -4016,7 +4029,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -4030,7 +4043,7 @@
       <c r="F85" s="34"/>
       <c r="G85" s="34"/>
     </row>
-    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B86" s="8" t="s">
         <v>14</v>
       </c>
@@ -4044,7 +4057,7 @@
       <c r="F86" s="34"/>
       <c r="G86" s="34"/>
     </row>
-    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B87" s="36" t="s">
         <v>14</v>
       </c>
@@ -4062,7 +4075,7 @@
       </c>
       <c r="G87" s="37"/>
     </row>
-    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B88" s="9" t="s">
         <v>15</v>
       </c>
@@ -4080,7 +4093,7 @@
       </c>
       <c r="G88" s="49"/>
     </row>
-    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B89" s="5" t="s">
         <v>12</v>
       </c>
@@ -4098,7 +4111,7 @@
       </c>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B90" s="5" t="s">
         <v>12</v>
       </c>
@@ -4116,7 +4129,7 @@
       </c>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B91" s="6" t="s">
         <v>13</v>
       </c>
@@ -4134,7 +4147,7 @@
       </c>
       <c r="G91" s="11"/>
     </row>
-    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B92" s="4" t="s">
         <v>9</v>
       </c>
@@ -4152,7 +4165,7 @@
       </c>
       <c r="G92" s="11"/>
     </row>
-    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B93" s="4" t="s">
         <v>9</v>
       </c>
@@ -4170,7 +4183,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" ht="15.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -4188,7 +4201,7 @@
       </c>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B95" s="4" t="s">
         <v>9</v>
       </c>
@@ -4206,7 +4219,7 @@
       </c>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B96" s="40" t="s">
         <v>15</v>
       </c>
@@ -4224,7 +4237,7 @@
       </c>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B97" s="10" t="s">
         <v>16</v>
       </c>
@@ -4242,7 +4255,7 @@
       </c>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B98" s="37" t="s">
         <v>150</v>
       </c>
@@ -4256,7 +4269,7 @@
       <c r="F98" s="37"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B99" s="5" t="s">
         <v>12</v>
       </c>
@@ -4274,7 +4287,7 @@
       </c>
       <c r="G99" s="11"/>
     </row>
-    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B100" s="5" t="s">
         <v>12</v>
       </c>
@@ -4290,7 +4303,7 @@
       </c>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B101" s="40" t="s">
         <v>15</v>
       </c>
@@ -4308,7 +4321,7 @@
       </c>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B102" s="6" t="s">
         <v>13</v>
       </c>
@@ -4324,7 +4337,7 @@
       </c>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B103" s="6" t="s">
         <v>13</v>
       </c>
@@ -4342,7 +4355,7 @@
       </c>
       <c r="G103" s="11"/>
     </row>
-    <row r="104" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B104" s="6" t="s">
         <v>13</v>
       </c>
@@ -4360,7 +4373,7 @@
       </c>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B105" s="42" t="s">
         <v>9</v>
       </c>
@@ -4378,7 +4391,7 @@
       </c>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B106" s="42" t="s">
         <v>9</v>
       </c>
@@ -4396,7 +4409,7 @@
       </c>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B107" s="42" t="s">
         <v>9</v>
       </c>
@@ -4414,7 +4427,7 @@
       </c>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B108" s="42" t="s">
         <v>9</v>
       </c>
@@ -4432,7 +4445,7 @@
       </c>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B109" s="42" t="s">
         <v>9</v>
       </c>
@@ -4450,7 +4463,7 @@
       </c>
       <c r="G109" s="11"/>
     </row>
-    <row r="110" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B110" s="42" t="s">
         <v>9</v>
       </c>
@@ -4468,7 +4481,7 @@
       </c>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B111" s="42" t="s">
         <v>9</v>
       </c>
@@ -4486,7 +4499,7 @@
       </c>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B112" s="43" t="s">
         <v>14</v>
       </c>
@@ -4500,7 +4513,7 @@
       <c r="F112" s="34"/>
       <c r="G112" s="34"/>
     </row>
-    <row r="113" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B113" s="44" t="s">
         <v>14</v>
       </c>
@@ -4514,7 +4527,7 @@
       <c r="F113" s="34"/>
       <c r="G113" s="34"/>
     </row>
-    <row r="114" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B114" s="44" t="s">
         <v>14</v>
       </c>
@@ -4528,7 +4541,7 @@
       <c r="F114" s="34"/>
       <c r="G114" s="34"/>
     </row>
-    <row r="115" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B115" s="5" t="s">
         <v>12</v>
       </c>
@@ -4546,7 +4559,7 @@
       </c>
       <c r="G115" s="11"/>
     </row>
-    <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B116" s="5" t="s">
         <v>12</v>
       </c>
@@ -4564,7 +4577,7 @@
       </c>
       <c r="G116" s="11"/>
     </row>
-    <row r="117" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B117" s="5" t="s">
         <v>12</v>
       </c>
@@ -4582,7 +4595,7 @@
       </c>
       <c r="G117" s="11"/>
     </row>
-    <row r="118" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B118" s="45" t="s">
         <v>13</v>
       </c>
@@ -4600,7 +4613,7 @@
       </c>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B119" s="45" t="s">
         <v>13</v>
       </c>
@@ -4618,7 +4631,7 @@
       </c>
       <c r="G119" s="11"/>
     </row>
-    <row r="120" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B120" s="45" t="s">
         <v>13</v>
       </c>
@@ -4634,7 +4647,7 @@
       </c>
       <c r="G120" s="11"/>
     </row>
-    <row r="121" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B121" s="10" t="s">
         <v>16</v>
       </c>
@@ -4642,7 +4655,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B122" s="4" t="s">
         <v>9</v>
       </c>
@@ -4660,7 +4673,7 @@
       </c>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B123" s="4" t="s">
         <v>9</v>
       </c>
@@ -4678,7 +4691,7 @@
       </c>
       <c r="G123" s="48"/>
     </row>
-    <row r="124" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B124" s="4" t="s">
         <v>9</v>
       </c>
@@ -4696,7 +4709,7 @@
       </c>
       <c r="G124" s="7"/>
     </row>
-    <row r="125" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B125" s="10" t="s">
         <v>16</v>
       </c>
@@ -4708,7 +4721,7 @@
       </c>
       <c r="G125" s="7"/>
     </row>
-    <row r="126" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B126" s="10" t="s">
         <v>16</v>
       </c>
@@ -4723,17 +4736,17 @@
       </c>
       <c r="G126" s="50"/>
     </row>
-    <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="63" t="s">
+    <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="64"/>
-      <c r="D127" s="64"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="64"/>
-      <c r="G127" s="64"/>
-    </row>
-    <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
+    </row>
+    <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B128" s="67"/>
       <c r="C128" s="68"/>
       <c r="D128" s="68"/>
@@ -4741,7 +4754,7 @@
       <c r="F128" s="68"/>
       <c r="G128" s="68"/>
     </row>
-    <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B129" s="51" t="s">
         <v>15</v>
       </c>
@@ -4766,7 +4779,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B130" s="51" t="s">
         <v>15</v>
       </c>
@@ -4793,7 +4806,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B131" s="52" t="s">
         <v>13</v>
       </c>
@@ -4820,7 +4833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B132" s="52" t="s">
         <v>13</v>
       </c>
@@ -4847,7 +4860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B133" s="53" t="s">
         <v>16</v>
       </c>
@@ -4872,7 +4885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B134" s="55" t="s">
         <v>12</v>
       </c>
@@ -4901,7 +4914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B135" s="56" t="s">
         <v>14</v>
       </c>
@@ -4924,7 +4937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B136" s="56" t="s">
         <v>14</v>
       </c>
@@ -4938,7 +4951,7 @@
       </c>
       <c r="G136" s="11"/>
     </row>
-    <row r="137" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B137" s="54" t="s">
         <v>9</v>
       </c>
@@ -4956,7 +4969,7 @@
       </c>
       <c r="G137" s="11"/>
     </row>
-    <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B138" s="54" t="s">
         <v>9</v>
       </c>
@@ -4974,7 +4987,7 @@
       </c>
       <c r="G138" s="7"/>
     </row>
-    <row r="139" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B139" s="54" t="s">
         <v>9</v>
       </c>
@@ -4992,7 +5005,7 @@
       </c>
       <c r="G139" s="7"/>
     </row>
-    <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B140" s="54" t="s">
         <v>9</v>
       </c>
@@ -5010,7 +5023,7 @@
       </c>
       <c r="G140" s="7"/>
     </row>
-    <row r="141" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B141" s="53" t="s">
         <v>16</v>
       </c>
@@ -5026,17 +5039,17 @@
       </c>
       <c r="G141" s="7"/>
     </row>
-    <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="63" t="s">
+    <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="64"/>
-      <c r="D142" s="64"/>
-      <c r="E142" s="64"/>
-      <c r="F142" s="64"/>
-      <c r="G142" s="64"/>
-    </row>
-    <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
+    </row>
+    <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B143" s="67"/>
       <c r="C143" s="68"/>
       <c r="D143" s="68"/>
@@ -5044,7 +5057,7 @@
       <c r="F143" s="68"/>
       <c r="G143" s="68"/>
     </row>
-    <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B144" s="55" t="s">
         <v>12</v>
       </c>
@@ -5071,7 +5084,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="145" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B145" s="55" t="s">
         <v>12</v>
       </c>
@@ -5100,7 +5113,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B146" s="53" t="s">
         <v>16</v>
       </c>
@@ -5109,8 +5122,10 @@
       </c>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
-      <c r="F146" s="13"/>
-      <c r="G146" s="13"/>
+      <c r="F146" s="13">
+        <v>3</v>
+      </c>
+      <c r="G146" s="83"/>
       <c r="I146" s="6" t="s">
         <v>13</v>
       </c>
@@ -5123,7 +5138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B147" s="55" t="s">
         <v>12</v>
       </c>
@@ -5142,7 +5157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B148" s="52" t="s">
         <v>13</v>
       </c>
@@ -5171,7 +5186,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B149" s="52" t="s">
         <v>13</v>
       </c>
@@ -5196,7 +5211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B150" s="52" t="s">
         <v>13</v>
       </c>
@@ -5213,7 +5228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B151" s="52" t="s">
         <v>13</v>
       </c>
@@ -5231,7 +5246,7 @@
       </c>
       <c r="G151" s="11"/>
     </row>
-    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B152" s="54" t="s">
         <v>9</v>
       </c>
@@ -5249,7 +5264,7 @@
       </c>
       <c r="G152" s="11"/>
     </row>
-    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B153" s="54" t="s">
         <v>9</v>
       </c>
@@ -5267,7 +5282,7 @@
       </c>
       <c r="G153" s="7"/>
     </row>
-    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B154" s="54" t="s">
         <v>9</v>
       </c>
@@ -5283,7 +5298,7 @@
       <c r="F154" s="13"/>
       <c r="G154" s="26"/>
     </row>
-    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B155" s="51" t="s">
         <v>15</v>
       </c>
@@ -5299,7 +5314,7 @@
       </c>
       <c r="G155" s="11"/>
     </row>
-    <row r="156" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B156" s="51" t="s">
         <v>15</v>
       </c>
@@ -5313,7 +5328,7 @@
       <c r="F156" s="13"/>
       <c r="G156" s="11"/>
     </row>
-    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B157" s="56" t="s">
         <v>14</v>
       </c>
@@ -5329,7 +5344,7 @@
       </c>
       <c r="G157" s="11"/>
     </row>
-    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B158" s="56" t="s">
         <v>14</v>
       </c>
@@ -5345,17 +5360,17 @@
       </c>
       <c r="G158" s="7"/>
     </row>
-    <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="63" t="s">
+    <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B159" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="64"/>
-      <c r="D159" s="64"/>
-      <c r="E159" s="64"/>
-      <c r="F159" s="64"/>
-      <c r="G159" s="64"/>
-    </row>
-    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C159" s="60"/>
+      <c r="D159" s="60"/>
+      <c r="E159" s="60"/>
+      <c r="F159" s="60"/>
+      <c r="G159" s="60"/>
+    </row>
+    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B160" s="67"/>
       <c r="C160" s="68"/>
       <c r="D160" s="68"/>
@@ -5372,7 +5387,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="161" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B161" s="56" t="s">
         <v>14</v>
       </c>
@@ -5399,7 +5414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B162" s="56" t="s">
         <v>14</v>
       </c>
@@ -5420,7 +5435,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B163" s="56" t="s">
         <v>14</v>
       </c>
@@ -5439,7 +5454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B164" s="56" t="s">
         <v>14</v>
       </c>
@@ -5461,7 +5476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B165" s="55" t="s">
         <v>12</v>
       </c>
@@ -5484,7 +5499,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B166" s="55" t="s">
         <v>12</v>
       </c>
@@ -5502,8 +5517,16 @@
       <c r="I166" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="167" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J166">
+        <f>F177+F178+F183</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="K166">
+        <f>F163+F164+F169</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="167" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B167" s="54" t="s">
         <v>9</v>
       </c>
@@ -5519,7 +5542,7 @@
       </c>
       <c r="G167" s="7"/>
     </row>
-    <row r="168" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B168" s="54" t="s">
         <v>9</v>
       </c>
@@ -5535,7 +5558,7 @@
       </c>
       <c r="G168" s="7"/>
     </row>
-    <row r="169" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B169" s="54" t="s">
         <v>9</v>
       </c>
@@ -5553,7 +5576,7 @@
       </c>
       <c r="G169" s="7"/>
     </row>
-    <row r="170" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B170" s="54" t="s">
         <v>9</v>
       </c>
@@ -5571,7 +5594,7 @@
       </c>
       <c r="G170" s="7"/>
     </row>
-    <row r="171" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B171" s="54" t="s">
         <v>9</v>
       </c>
@@ -5589,7 +5612,7 @@
       </c>
       <c r="G171" s="7"/>
     </row>
-    <row r="172" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B172" s="54" t="s">
         <v>9</v>
       </c>
@@ -5607,7 +5630,7 @@
       </c>
       <c r="G172" s="7"/>
     </row>
-    <row r="173" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B173" s="52" t="s">
         <v>13</v>
       </c>
@@ -5625,7 +5648,7 @@
       </c>
       <c r="G173" s="11"/>
     </row>
-    <row r="174" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B174" s="52" t="s">
         <v>13</v>
       </c>
@@ -5643,7 +5666,7 @@
       </c>
       <c r="G174" s="7"/>
     </row>
-    <row r="175" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B175" s="52" t="s">
         <v>13</v>
       </c>
@@ -5661,7 +5684,7 @@
       </c>
       <c r="G175" s="11"/>
     </row>
-    <row r="176" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B176" s="52" t="s">
         <v>13</v>
       </c>
@@ -5677,7 +5700,7 @@
       </c>
       <c r="G176" s="50"/>
     </row>
-    <row r="177" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B177" s="53" t="s">
         <v>16</v>
       </c>
@@ -5685,21 +5708,29 @@
         <v>213</v>
       </c>
       <c r="D177" s="13"/>
-      <c r="E177" s="13"/>
-      <c r="F177" s="13"/>
-      <c r="G177" s="1"/>
-    </row>
-    <row r="178" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E177" s="13">
+        <v>6</v>
+      </c>
+      <c r="F177" s="13">
+        <v>10.6</v>
+      </c>
+      <c r="G177" s="82"/>
+    </row>
+    <row r="178" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B178" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="C178" s="13"/>
+      <c r="C178" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
-      <c r="F178" s="13"/>
-      <c r="G178" s="1"/>
-    </row>
-    <row r="179" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F178" s="13">
+        <v>7</v>
+      </c>
+      <c r="G178" s="82"/>
+    </row>
+    <row r="179" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B179" s="51" t="s">
         <v>15</v>
       </c>
@@ -5711,7 +5742,7 @@
       <c r="F179" s="13"/>
       <c r="G179" s="1"/>
     </row>
-    <row r="180" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B180" s="51" t="s">
         <v>15</v>
       </c>
@@ -5723,7 +5754,7 @@
       <c r="F180" s="13"/>
       <c r="G180" s="1"/>
     </row>
-    <row r="181" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B181" s="55" t="s">
         <v>12</v>
       </c>
@@ -5739,7 +5770,7 @@
       </c>
       <c r="G181" s="7"/>
     </row>
-    <row r="182" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B182" s="52" t="s">
         <v>13</v>
       </c>
@@ -5753,8 +5784,24 @@
       </c>
       <c r="G182" s="11"/>
     </row>
+    <row r="183" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B183" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C183" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="13">
+        <v>0</v>
+      </c>
+      <c r="G183" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="J22:L22"/>
@@ -5771,8 +5818,6 @@
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
     <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
-    <mergeCell ref="B159:G160"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5792,17 +5837,17 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.52734375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.52734375" customWidth="1"/>
+    <col min="2" max="2" width="35.46875" customWidth="1"/>
+    <col min="3" max="3" width="27.46875" customWidth="1"/>
+    <col min="4" max="4" width="10.46875" customWidth="1"/>
+    <col min="7" max="7" width="17.46875" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
         <v>91</v>
       </c>
@@ -5832,7 +5877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -5861,7 +5906,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -5884,7 +5929,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -5907,7 +5952,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -5922,7 +5967,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -5941,7 +5986,7 @@
       </c>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -5964,7 +6009,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -5979,7 +6024,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -6002,7 +6047,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -6017,7 +6062,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -6032,7 +6077,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -6049,7 +6094,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -6064,7 +6109,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -6081,7 +6126,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -6096,7 +6141,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -6111,7 +6156,7 @@
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -6126,7 +6171,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -6149,7 +6194,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -6172,7 +6217,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -6186,7 +6231,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -6207,7 +6252,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -6222,7 +6267,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -6237,7 +6282,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -6258,7 +6303,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -6273,7 +6318,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -6296,7 +6341,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -6311,7 +6356,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -6334,7 +6379,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -6349,7 +6394,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -6366,7 +6411,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -6389,7 +6434,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -6410,7 +6455,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -6431,7 +6476,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -6454,7 +6499,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -6471,7 +6516,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -6486,7 +6531,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -6509,7 +6554,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -6526,7 +6571,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -6541,7 +6586,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -6562,7 +6607,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -6585,7 +6630,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -6608,7 +6653,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -6631,7 +6676,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -6654,7 +6699,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -6675,7 +6720,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -6692,7 +6737,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -6713,7 +6758,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="15">
         <v>47</v>
       </c>
@@ -6736,7 +6781,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="38">
         <v>48</v>
       </c>
@@ -6762,23 +6807,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6987,10 +7015,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7013,20 +7069,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>